<commit_message>
FEAT: Añadir carga de datos para condiciones de vulnerabilidad, indicadores de valoración y tipos de actividad en el comando de población de base de datos
</commit_message>
<xml_diff>
--- a/runna/infrastructure/management/fixtures/localidades prov cba.xlsx
+++ b/runna/infrastructure/management/fixtures/localidades prov cba.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="461">
   <si>
     <t>ID</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>INTERIOR</t>
-  </si>
-  <si>
-    <t>PRUEBALOCAL1</t>
   </si>
   <si>
     <t>DEL CAMPILLO</t>
@@ -1531,10 +1528,10 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1838,7 +1835,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B999"/>
+  <dimension ref="A1:B998"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1930,15 +1927,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A11" s="4">
-        <v>490</v>
+        <v>2</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A12" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>2</v>
@@ -1946,15 +1943,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A13" s="4">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A14" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>7</v>
@@ -1962,7 +1959,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A15" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>8</v>
@@ -1970,7 +1967,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A16" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>9</v>
@@ -1978,7 +1975,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A17" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>10</v>
@@ -1986,7 +1983,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>11</v>
@@ -1994,7 +1991,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>12</v>
@@ -2002,7 +1999,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>13</v>
@@ -2010,7 +2007,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>14</v>
@@ -2018,7 +2015,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A22" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>15</v>
@@ -2026,7 +2023,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A23" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>16</v>
@@ -2034,7 +2031,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A24" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>17</v>
@@ -2042,7 +2039,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A25" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>18</v>
@@ -2050,7 +2047,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A26" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>19</v>
@@ -2058,7 +2055,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A27" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>20</v>
@@ -2066,7 +2063,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A28" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>21</v>
@@ -2074,7 +2071,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A29" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>22</v>
@@ -2082,7 +2079,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A30" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>23</v>
@@ -2090,7 +2087,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A31" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>24</v>
@@ -2098,7 +2095,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A32" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>25</v>
@@ -2106,7 +2103,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A33" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>26</v>
@@ -2114,7 +2111,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A34" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>27</v>
@@ -2122,7 +2119,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A35" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>28</v>
@@ -2130,7 +2127,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A36" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>29</v>
@@ -2138,7 +2135,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A37" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>30</v>
@@ -2146,7 +2143,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A38" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>31</v>
@@ -2154,7 +2151,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A39" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>32</v>
@@ -2162,7 +2159,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A40" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>33</v>
@@ -2170,7 +2167,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A41" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>34</v>
@@ -2178,7 +2175,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A42" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>35</v>
@@ -2186,7 +2183,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A43" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>36</v>
@@ -2194,7 +2191,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A44" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>37</v>
@@ -2202,7 +2199,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A45" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>38</v>
@@ -2210,7 +2207,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A46" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>39</v>
@@ -2218,7 +2215,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A47" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>40</v>
@@ -2226,7 +2223,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A48" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>41</v>
@@ -2234,7 +2231,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A49" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>42</v>
@@ -2242,7 +2239,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A50" s="4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>43</v>
@@ -2250,7 +2247,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A51" s="4">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>44</v>
@@ -2258,7 +2255,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A52" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>45</v>
@@ -2266,7 +2263,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A53" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>46</v>
@@ -2274,7 +2271,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A54" s="4">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>47</v>
@@ -2282,7 +2279,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A55" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>48</v>
@@ -2290,7 +2287,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A56" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>49</v>
@@ -2298,7 +2295,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A57" s="4">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>50</v>
@@ -2306,7 +2303,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A58" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>51</v>
@@ -2314,7 +2311,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A59" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>52</v>
@@ -2322,7 +2319,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A60" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>53</v>
@@ -2330,7 +2327,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A61" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>54</v>
@@ -2338,7 +2335,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A62" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>55</v>
@@ -2346,7 +2343,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A63" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>56</v>
@@ -2354,7 +2351,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A64" s="4">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>57</v>
@@ -2362,7 +2359,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A65" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>58</v>
@@ -2370,7 +2367,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A66" s="4">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>59</v>
@@ -2378,7 +2375,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A67" s="4">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>60</v>
@@ -2386,7 +2383,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A68" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>61</v>
@@ -2394,7 +2391,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A69" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>62</v>
@@ -2402,7 +2399,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A70" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>63</v>
@@ -2410,7 +2407,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A71" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>64</v>
@@ -2418,7 +2415,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A72" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>65</v>
@@ -2426,7 +2423,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A73" s="4">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>66</v>
@@ -2434,7 +2431,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A74" s="4">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>67</v>
@@ -2442,7 +2439,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A75" s="4">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>68</v>
@@ -2450,7 +2447,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A76" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>69</v>
@@ -2458,7 +2455,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A77" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>70</v>
@@ -2466,7 +2463,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A78" s="4">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>71</v>
@@ -2474,7 +2471,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A79" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>72</v>
@@ -2482,7 +2479,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A80" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>73</v>
@@ -2490,7 +2487,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A81" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>74</v>
@@ -2498,7 +2495,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A82" s="4">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>75</v>
@@ -2506,7 +2503,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A83" s="4">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>76</v>
@@ -2514,7 +2511,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A84" s="4">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>77</v>
@@ -2522,7 +2519,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A85" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>78</v>
@@ -2530,7 +2527,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A86" s="4">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>79</v>
@@ -2538,7 +2535,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A87" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>80</v>
@@ -2546,7 +2543,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A88" s="4">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>81</v>
@@ -2554,7 +2551,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A89" s="4">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>82</v>
@@ -2562,7 +2559,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A90" s="4">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>83</v>
@@ -2570,7 +2567,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A91" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>84</v>
@@ -2578,7 +2575,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A92" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>85</v>
@@ -2586,7 +2583,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A93" s="4">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>86</v>
@@ -2594,7 +2591,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A94" s="4">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>87</v>
@@ -2602,7 +2599,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A95" s="4">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>88</v>
@@ -2610,7 +2607,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A96" s="4">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>89</v>
@@ -2618,7 +2615,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A97" s="4">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>90</v>
@@ -2626,7 +2623,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A98" s="4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>91</v>
@@ -2634,7 +2631,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A99" s="4">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>92</v>
@@ -2642,7 +2639,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A100" s="4">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>93</v>
@@ -2650,7 +2647,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A101" s="4">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>94</v>
@@ -2658,7 +2655,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A102" s="4">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>95</v>
@@ -2666,7 +2663,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A103" s="4">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>96</v>
@@ -2674,7 +2671,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A104" s="4">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>97</v>
@@ -2682,7 +2679,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A105" s="4">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>98</v>
@@ -2690,7 +2687,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A106" s="4">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>99</v>
@@ -2698,7 +2695,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A107" s="4">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>100</v>
@@ -2706,7 +2703,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A108" s="4">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>101</v>
@@ -2714,7 +2711,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A109" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>102</v>
@@ -2722,7 +2719,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A110" s="4">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>103</v>
@@ -2730,7 +2727,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A111" s="4">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>104</v>
@@ -2738,7 +2735,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A112" s="4">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>105</v>
@@ -2746,7 +2743,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A113" s="4">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>106</v>
@@ -2754,7 +2751,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A114" s="4">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>107</v>
@@ -2762,7 +2759,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A115" s="4">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>108</v>
@@ -2770,7 +2767,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A116" s="4">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>109</v>
@@ -2778,7 +2775,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A117" s="4">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>110</v>
@@ -2786,7 +2783,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A118" s="4">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>111</v>
@@ -2794,7 +2791,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A119" s="4">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>112</v>
@@ -2802,7 +2799,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A120" s="4">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>113</v>
@@ -2810,7 +2807,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A121" s="4">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>114</v>
@@ -2818,7 +2815,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A122" s="4">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>115</v>
@@ -2826,7 +2823,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A123" s="4">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>116</v>
@@ -2834,7 +2831,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A124" s="4">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>117</v>
@@ -2842,7 +2839,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A125" s="4">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>118</v>
@@ -2850,7 +2847,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A126" s="4">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>119</v>
@@ -2858,7 +2855,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A127" s="4">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>120</v>
@@ -2866,7 +2863,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A128" s="4">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>121</v>
@@ -2874,7 +2871,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A129" s="4">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>122</v>
@@ -2882,7 +2879,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A130" s="4">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>123</v>
@@ -2890,7 +2887,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A131" s="4">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>124</v>
@@ -2898,7 +2895,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A132" s="4">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>125</v>
@@ -2906,7 +2903,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A133" s="4">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>126</v>
@@ -2914,7 +2911,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A134" s="4">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>127</v>
@@ -2922,7 +2919,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A135" s="4">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>128</v>
@@ -2930,7 +2927,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A136" s="4">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>129</v>
@@ -2938,7 +2935,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A137" s="4">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>130</v>
@@ -2946,7 +2943,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A138" s="4">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>131</v>
@@ -2954,7 +2951,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A139" s="4">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B139" s="5" t="s">
         <v>132</v>
@@ -2962,7 +2959,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A140" s="4">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>133</v>
@@ -2970,7 +2967,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A141" s="4">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>134</v>
@@ -2978,7 +2975,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A142" s="4">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>135</v>
@@ -2986,7 +2983,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A143" s="4">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B143" s="5" t="s">
         <v>136</v>
@@ -2994,7 +2991,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A144" s="4">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B144" s="5" t="s">
         <v>137</v>
@@ -3002,7 +2999,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A145" s="4">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B145" s="5" t="s">
         <v>138</v>
@@ -3010,7 +3007,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A146" s="4">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B146" s="5" t="s">
         <v>139</v>
@@ -3018,7 +3015,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A147" s="4">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>140</v>
@@ -3026,7 +3023,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A148" s="4">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>141</v>
@@ -3034,7 +3031,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A149" s="4">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>142</v>
@@ -3042,7 +3039,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A150" s="4">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>143</v>
@@ -3050,7 +3047,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A151" s="4">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>144</v>
@@ -3058,7 +3055,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A152" s="4">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>145</v>
@@ -3066,7 +3063,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A153" s="4">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B153" s="5" t="s">
         <v>146</v>
@@ -3074,7 +3071,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A154" s="4">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>147</v>
@@ -3082,7 +3079,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A155" s="4">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B155" s="5" t="s">
         <v>148</v>
@@ -3090,7 +3087,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A156" s="4">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B156" s="5" t="s">
         <v>149</v>
@@ -3098,7 +3095,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A157" s="4">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>150</v>
@@ -3106,7 +3103,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A158" s="4">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>151</v>
@@ -3114,7 +3111,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A159" s="4">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>152</v>
@@ -3122,7 +3119,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A160" s="4">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>153</v>
@@ -3130,7 +3127,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A161" s="4">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>154</v>
@@ -3138,7 +3135,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A162" s="4">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>155</v>
@@ -3146,7 +3143,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A163" s="4">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>156</v>
@@ -3154,7 +3151,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A164" s="4">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>157</v>
@@ -3162,7 +3159,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A165" s="4">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>158</v>
@@ -3170,7 +3167,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A166" s="4">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>159</v>
@@ -3178,7 +3175,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A167" s="4">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>160</v>
@@ -3186,7 +3183,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A168" s="4">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>161</v>
@@ -3194,7 +3191,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A169" s="4">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="B169" s="5" t="s">
         <v>162</v>
@@ -3202,7 +3199,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A170" s="4">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B170" s="5" t="s">
         <v>163</v>
@@ -3210,7 +3207,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A171" s="4">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B171" s="5" t="s">
         <v>164</v>
@@ -3218,7 +3215,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A172" s="4">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B172" s="5" t="s">
         <v>165</v>
@@ -3226,7 +3223,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A173" s="4">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B173" s="5" t="s">
         <v>166</v>
@@ -3234,7 +3231,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A174" s="4">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B174" s="5" t="s">
         <v>167</v>
@@ -3242,7 +3239,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A175" s="4">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>168</v>
@@ -3250,7 +3247,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A176" s="4">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B176" s="5" t="s">
         <v>169</v>
@@ -3258,7 +3255,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A177" s="4">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B177" s="5" t="s">
         <v>170</v>
@@ -3266,7 +3263,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A178" s="4">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B178" s="5" t="s">
         <v>171</v>
@@ -3274,7 +3271,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A179" s="4">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B179" s="5" t="s">
         <v>172</v>
@@ -3282,7 +3279,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A180" s="4">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B180" s="5" t="s">
         <v>173</v>
@@ -3290,7 +3287,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A181" s="4">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>174</v>
@@ -3298,7 +3295,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A182" s="4">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B182" s="5" t="s">
         <v>175</v>
@@ -3306,7 +3303,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A183" s="4">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B183" s="5" t="s">
         <v>176</v>
@@ -3314,7 +3311,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A184" s="4">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B184" s="5" t="s">
         <v>177</v>
@@ -3322,7 +3319,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A185" s="4">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B185" s="5" t="s">
         <v>178</v>
@@ -3330,7 +3327,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A186" s="4">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B186" s="5" t="s">
         <v>179</v>
@@ -3338,7 +3335,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A187" s="4">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B187" s="5" t="s">
         <v>180</v>
@@ -3346,7 +3343,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A188" s="4">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B188" s="5" t="s">
         <v>181</v>
@@ -3354,7 +3351,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A189" s="4">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B189" s="5" t="s">
         <v>182</v>
@@ -3362,7 +3359,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A190" s="4">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B190" s="5" t="s">
         <v>183</v>
@@ -3370,7 +3367,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A191" s="4">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B191" s="5" t="s">
         <v>184</v>
@@ -3378,7 +3375,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A192" s="4">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B192" s="5" t="s">
         <v>185</v>
@@ -3386,7 +3383,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A193" s="4">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B193" s="5" t="s">
         <v>186</v>
@@ -3394,7 +3391,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A194" s="4">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B194" s="5" t="s">
         <v>187</v>
@@ -3402,7 +3399,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A195" s="4">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B195" s="5" t="s">
         <v>188</v>
@@ -3410,7 +3407,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A196" s="4">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B196" s="5" t="s">
         <v>189</v>
@@ -3418,7 +3415,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A197" s="4">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B197" s="5" t="s">
         <v>190</v>
@@ -3426,7 +3423,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A198" s="4">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B198" s="5" t="s">
         <v>191</v>
@@ -3434,7 +3431,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A199" s="4">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B199" s="5" t="s">
         <v>192</v>
@@ -3442,7 +3439,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A200" s="4">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B200" s="5" t="s">
         <v>193</v>
@@ -3450,7 +3447,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A201" s="4">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B201" s="5" t="s">
         <v>194</v>
@@ -3458,7 +3455,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A202" s="4">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B202" s="5" t="s">
         <v>195</v>
@@ -3466,7 +3463,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A203" s="4">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B203" s="5" t="s">
         <v>196</v>
@@ -3474,7 +3471,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A204" s="4">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B204" s="5" t="s">
         <v>197</v>
@@ -3482,7 +3479,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A205" s="4">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B205" s="5" t="s">
         <v>198</v>
@@ -3490,7 +3487,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A206" s="4">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="B206" s="5" t="s">
         <v>199</v>
@@ -3498,7 +3495,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A207" s="4">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B207" s="5" t="s">
         <v>200</v>
@@ -3506,7 +3503,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A208" s="4">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B208" s="5" t="s">
         <v>201</v>
@@ -3514,7 +3511,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A209" s="4">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B209" s="5" t="s">
         <v>202</v>
@@ -3522,7 +3519,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A210" s="4">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B210" s="5" t="s">
         <v>203</v>
@@ -3530,7 +3527,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A211" s="4">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B211" s="5" t="s">
         <v>204</v>
@@ -3538,7 +3535,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A212" s="4">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B212" s="5" t="s">
         <v>205</v>
@@ -3546,7 +3543,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A213" s="4">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B213" s="5" t="s">
         <v>206</v>
@@ -3554,7 +3551,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A214" s="4">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B214" s="5" t="s">
         <v>207</v>
@@ -3562,7 +3559,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A215" s="4">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B215" s="5" t="s">
         <v>208</v>
@@ -3570,7 +3567,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A216" s="4">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B216" s="5" t="s">
         <v>209</v>
@@ -3578,7 +3575,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A217" s="4">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B217" s="5" t="s">
         <v>210</v>
@@ -3586,7 +3583,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A218" s="4">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B218" s="5" t="s">
         <v>211</v>
@@ -3594,7 +3591,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A219" s="4">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B219" s="5" t="s">
         <v>212</v>
@@ -3602,7 +3599,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A220" s="4">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B220" s="5" t="s">
         <v>213</v>
@@ -3610,7 +3607,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A221" s="4">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B221" s="5" t="s">
         <v>214</v>
@@ -3618,7 +3615,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A222" s="4">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B222" s="5" t="s">
         <v>215</v>
@@ -3626,7 +3623,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A223" s="4">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B223" s="5" t="s">
         <v>216</v>
@@ -3634,7 +3631,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A224" s="4">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B224" s="5" t="s">
         <v>217</v>
@@ -3642,7 +3639,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A225" s="4">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B225" s="5" t="s">
         <v>218</v>
@@ -3650,7 +3647,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A226" s="4">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B226" s="5" t="s">
         <v>219</v>
@@ -3658,7 +3655,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A227" s="4">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B227" s="5" t="s">
         <v>220</v>
@@ -3666,7 +3663,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A228" s="4">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B228" s="5" t="s">
         <v>221</v>
@@ -3674,7 +3671,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A229" s="4">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B229" s="5" t="s">
         <v>222</v>
@@ -3682,7 +3679,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A230" s="4">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B230" s="5" t="s">
         <v>223</v>
@@ -3690,7 +3687,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A231" s="4">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B231" s="5" t="s">
         <v>224</v>
@@ -3698,7 +3695,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A232" s="4">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B232" s="5" t="s">
         <v>225</v>
@@ -3706,7 +3703,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A233" s="4">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B233" s="5" t="s">
         <v>226</v>
@@ -3714,7 +3711,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A234" s="4">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B234" s="5" t="s">
         <v>227</v>
@@ -3722,7 +3719,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A235" s="4">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B235" s="5" t="s">
         <v>228</v>
@@ -3730,7 +3727,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A236" s="4">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B236" s="5" t="s">
         <v>229</v>
@@ -3738,7 +3735,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A237" s="4">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B237" s="5" t="s">
         <v>230</v>
@@ -3746,7 +3743,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A238" s="4">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B238" s="5" t="s">
         <v>231</v>
@@ -3754,7 +3751,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A239" s="4">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B239" s="5" t="s">
         <v>232</v>
@@ -3762,7 +3759,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A240" s="4">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B240" s="5" t="s">
         <v>233</v>
@@ -3770,7 +3767,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A241" s="4">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B241" s="5" t="s">
         <v>234</v>
@@ -3778,7 +3775,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A242" s="4">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B242" s="5" t="s">
         <v>235</v>
@@ -3786,7 +3783,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A243" s="4">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B243" s="5" t="s">
         <v>236</v>
@@ -3794,7 +3791,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A244" s="4">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B244" s="5" t="s">
         <v>237</v>
@@ -3802,7 +3799,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A245" s="4">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B245" s="5" t="s">
         <v>238</v>
@@ -3810,7 +3807,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A246" s="4">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B246" s="5" t="s">
         <v>239</v>
@@ -3818,7 +3815,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A247" s="4">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B247" s="5" t="s">
         <v>240</v>
@@ -3826,7 +3823,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A248" s="4">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B248" s="5" t="s">
         <v>241</v>
@@ -3834,7 +3831,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A249" s="4">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B249" s="5" t="s">
         <v>242</v>
@@ -3842,7 +3839,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A250" s="4">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B250" s="5" t="s">
         <v>243</v>
@@ -3850,7 +3847,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A251" s="4">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B251" s="5" t="s">
         <v>244</v>
@@ -3858,7 +3855,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A252" s="4">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B252" s="5" t="s">
         <v>245</v>
@@ -3866,7 +3863,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A253" s="4">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B253" s="5" t="s">
         <v>246</v>
@@ -3874,7 +3871,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A254" s="4">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B254" s="5" t="s">
         <v>247</v>
@@ -3882,7 +3879,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A255" s="4">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B255" s="5" t="s">
         <v>248</v>
@@ -3890,7 +3887,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A256" s="4">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B256" s="5" t="s">
         <v>249</v>
@@ -3898,7 +3895,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A257" s="4">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B257" s="5" t="s">
         <v>250</v>
@@ -3906,7 +3903,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A258" s="4">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B258" s="5" t="s">
         <v>251</v>
@@ -3914,7 +3911,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A259" s="4">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B259" s="5" t="s">
         <v>252</v>
@@ -3922,7 +3919,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A260" s="4">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B260" s="5" t="s">
         <v>253</v>
@@ -3930,7 +3927,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="261" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A261" s="4">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B261" s="5" t="s">
         <v>254</v>
@@ -3938,7 +3935,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="262" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A262" s="4">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B262" s="5" t="s">
         <v>255</v>
@@ -3946,7 +3943,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="263" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A263" s="4">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B263" s="5" t="s">
         <v>256</v>
@@ -3954,7 +3951,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="264" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A264" s="4">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B264" s="5" t="s">
         <v>257</v>
@@ -3962,7 +3959,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="265" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A265" s="4">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B265" s="5" t="s">
         <v>258</v>
@@ -3970,7 +3967,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="266" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A266" s="4">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B266" s="5" t="s">
         <v>259</v>
@@ -3978,7 +3975,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="267" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A267" s="4">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B267" s="5" t="s">
         <v>260</v>
@@ -3986,7 +3983,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="268" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A268" s="4">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B268" s="5" t="s">
         <v>261</v>
@@ -3994,7 +3991,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="269" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A269" s="4">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B269" s="5" t="s">
         <v>262</v>
@@ -4002,7 +3999,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="270" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A270" s="4">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B270" s="5" t="s">
         <v>263</v>
@@ -4010,7 +4007,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="271" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A271" s="4">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B271" s="5" t="s">
         <v>264</v>
@@ -4018,7 +4015,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="272" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A272" s="4">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B272" s="5" t="s">
         <v>265</v>
@@ -4026,7 +4023,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="273" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A273" s="4">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B273" s="5" t="s">
         <v>266</v>
@@ -4034,7 +4031,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="274" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A274" s="4">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B274" s="5" t="s">
         <v>267</v>
@@ -4042,7 +4039,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="275" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A275" s="4">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B275" s="5" t="s">
         <v>268</v>
@@ -4050,7 +4047,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="276" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A276" s="4">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B276" s="5" t="s">
         <v>269</v>
@@ -4058,7 +4055,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="277" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A277" s="4">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B277" s="5" t="s">
         <v>270</v>
@@ -4066,7 +4063,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="278" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A278" s="4">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B278" s="5" t="s">
         <v>271</v>
@@ -4074,7 +4071,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="279" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A279" s="4">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B279" s="5" t="s">
         <v>272</v>
@@ -4082,7 +4079,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="280" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A280" s="4">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B280" s="5" t="s">
         <v>273</v>
@@ -4090,7 +4087,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="281" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A281" s="4">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B281" s="5" t="s">
         <v>274</v>
@@ -4098,7 +4095,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="282" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A282" s="4">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B282" s="5" t="s">
         <v>275</v>
@@ -4106,7 +4103,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="283" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A283" s="4">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B283" s="5" t="s">
         <v>276</v>
@@ -4114,7 +4111,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="284" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A284" s="4">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B284" s="5" t="s">
         <v>277</v>
@@ -4122,7 +4119,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="285" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A285" s="4">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B285" s="5" t="s">
         <v>278</v>
@@ -4130,7 +4127,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="286" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A286" s="4">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B286" s="5" t="s">
         <v>279</v>
@@ -4138,7 +4135,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="287" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A287" s="4">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B287" s="5" t="s">
         <v>280</v>
@@ -4146,7 +4143,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="288" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A288" s="4">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B288" s="5" t="s">
         <v>281</v>
@@ -4154,7 +4151,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="289" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A289" s="4">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B289" s="5" t="s">
         <v>282</v>
@@ -4162,7 +4159,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="290" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A290" s="4">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B290" s="5" t="s">
         <v>283</v>
@@ -4170,7 +4167,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="291" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A291" s="4">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B291" s="5" t="s">
         <v>284</v>
@@ -4178,7 +4175,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="292" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A292" s="4">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B292" s="5" t="s">
         <v>285</v>
@@ -4186,7 +4183,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="293" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A293" s="4">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B293" s="5" t="s">
         <v>286</v>
@@ -4194,7 +4191,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="294" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A294" s="4">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B294" s="5" t="s">
         <v>287</v>
@@ -4202,7 +4199,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="295" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A295" s="4">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B295" s="5" t="s">
         <v>288</v>
@@ -4210,7 +4207,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="296" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A296" s="4">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B296" s="5" t="s">
         <v>289</v>
@@ -4218,7 +4215,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="297" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A297" s="4">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B297" s="5" t="s">
         <v>290</v>
@@ -4226,7 +4223,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="298" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A298" s="4">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B298" s="5" t="s">
         <v>291</v>
@@ -4234,7 +4231,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="299" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A299" s="4">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B299" s="5" t="s">
         <v>292</v>
@@ -4242,7 +4239,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="300" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A300" s="4">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B300" s="5" t="s">
         <v>293</v>
@@ -4250,7 +4247,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="301" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A301" s="4">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B301" s="5" t="s">
         <v>294</v>
@@ -4258,7 +4255,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="302" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A302" s="4">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B302" s="5" t="s">
         <v>295</v>
@@ -4266,7 +4263,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="303" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A303" s="4">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B303" s="5" t="s">
         <v>296</v>
@@ -4274,7 +4271,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="304" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A304" s="4">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B304" s="5" t="s">
         <v>297</v>
@@ -4282,7 +4279,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="305" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A305" s="4">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B305" s="5" t="s">
         <v>298</v>
@@ -4290,7 +4287,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="306" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A306" s="4">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B306" s="5" t="s">
         <v>299</v>
@@ -4298,7 +4295,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="307" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A307" s="4">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B307" s="5" t="s">
         <v>300</v>
@@ -4306,7 +4303,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="308" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A308" s="4">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B308" s="5" t="s">
         <v>301</v>
@@ -4314,7 +4311,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="309" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A309" s="4">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B309" s="5" t="s">
         <v>302</v>
@@ -4322,7 +4319,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="310" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A310" s="4">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B310" s="5" t="s">
         <v>303</v>
@@ -4330,7 +4327,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="311" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A311" s="4">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B311" s="5" t="s">
         <v>304</v>
@@ -4338,7 +4335,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="312" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A312" s="4">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B312" s="5" t="s">
         <v>305</v>
@@ -4346,7 +4343,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="313" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A313" s="4">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B313" s="5" t="s">
         <v>306</v>
@@ -4354,7 +4351,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="314" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A314" s="4">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B314" s="5" t="s">
         <v>307</v>
@@ -4362,7 +4359,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="315" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A315" s="4">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B315" s="5" t="s">
         <v>308</v>
@@ -4370,7 +4367,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="316" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A316" s="4">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B316" s="5" t="s">
         <v>309</v>
@@ -4378,7 +4375,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="317" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A317" s="4">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B317" s="5" t="s">
         <v>310</v>
@@ -4386,7 +4383,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="318" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A318" s="4">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B318" s="5" t="s">
         <v>311</v>
@@ -4394,7 +4391,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="319" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A319" s="4">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B319" s="5" t="s">
         <v>312</v>
@@ -4402,7 +4399,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="320" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A320" s="4">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B320" s="5" t="s">
         <v>313</v>
@@ -4410,7 +4407,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="321" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A321" s="4">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B321" s="5" t="s">
         <v>314</v>
@@ -4418,7 +4415,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="322" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A322" s="4">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B322" s="5" t="s">
         <v>315</v>
@@ -4426,7 +4423,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="323" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A323" s="4">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B323" s="5" t="s">
         <v>316</v>
@@ -4434,7 +4431,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="324" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A324" s="4">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B324" s="5" t="s">
         <v>317</v>
@@ -4442,7 +4439,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="325" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A325" s="4">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B325" s="5" t="s">
         <v>318</v>
@@ -4450,7 +4447,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="326" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A326" s="4">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B326" s="5" t="s">
         <v>319</v>
@@ -4458,7 +4455,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="327" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A327" s="4">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B327" s="5" t="s">
         <v>320</v>
@@ -4466,7 +4463,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="328" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A328" s="4">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B328" s="5" t="s">
         <v>321</v>
@@ -4474,7 +4471,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="329" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A329" s="4">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B329" s="5" t="s">
         <v>322</v>
@@ -4482,7 +4479,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="330" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A330" s="4">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B330" s="5" t="s">
         <v>323</v>
@@ -4490,7 +4487,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="331" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A331" s="4">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B331" s="5" t="s">
         <v>324</v>
@@ -4498,7 +4495,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="332" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A332" s="4">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B332" s="5" t="s">
         <v>325</v>
@@ -4506,7 +4503,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="333" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A333" s="4">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B333" s="5" t="s">
         <v>326</v>
@@ -4514,7 +4511,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="334" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A334" s="4">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B334" s="5" t="s">
         <v>327</v>
@@ -4522,7 +4519,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="335" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A335" s="4">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B335" s="5" t="s">
         <v>328</v>
@@ -4530,7 +4527,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="336" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A336" s="4">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B336" s="5" t="s">
         <v>329</v>
@@ -4538,7 +4535,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="337" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A337" s="4">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B337" s="5" t="s">
         <v>330</v>
@@ -4546,7 +4543,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="338" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A338" s="4">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B338" s="5" t="s">
         <v>331</v>
@@ -4554,7 +4551,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="339" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A339" s="4">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B339" s="5" t="s">
         <v>332</v>
@@ -4562,7 +4559,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="340" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A340" s="4">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B340" s="5" t="s">
         <v>333</v>
@@ -4570,7 +4567,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="341" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A341" s="4">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B341" s="5" t="s">
         <v>334</v>
@@ -4578,7 +4575,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="342" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A342" s="4">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B342" s="5" t="s">
         <v>335</v>
@@ -4586,7 +4583,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="343" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A343" s="4">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B343" s="5" t="s">
         <v>336</v>
@@ -4594,7 +4591,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="344" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A344" s="4">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B344" s="5" t="s">
         <v>337</v>
@@ -4602,7 +4599,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="345" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A345" s="4">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B345" s="5" t="s">
         <v>338</v>
@@ -4610,7 +4607,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="346" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A346" s="4">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B346" s="5" t="s">
         <v>339</v>
@@ -4618,7 +4615,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="347" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A347" s="4">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B347" s="5" t="s">
         <v>340</v>
@@ -4626,7 +4623,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="348" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A348" s="4">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B348" s="5" t="s">
         <v>341</v>
@@ -4634,7 +4631,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="349" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A349" s="4">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B349" s="5" t="s">
         <v>342</v>
@@ -4642,7 +4639,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="350" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A350" s="4">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B350" s="5" t="s">
         <v>343</v>
@@ -4650,7 +4647,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="351" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A351" s="4">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B351" s="5" t="s">
         <v>344</v>
@@ -4658,7 +4655,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="352" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A352" s="4">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B352" s="5" t="s">
         <v>345</v>
@@ -4666,7 +4663,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="353" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A353" s="4">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B353" s="5" t="s">
         <v>346</v>
@@ -4674,7 +4671,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="354" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A354" s="4">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B354" s="5" t="s">
         <v>347</v>
@@ -4682,7 +4679,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="355" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A355" s="4">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B355" s="5" t="s">
         <v>348</v>
@@ -4690,7 +4687,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="356" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A356" s="4">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B356" s="5" t="s">
         <v>349</v>
@@ -4698,7 +4695,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="357" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A357" s="4">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B357" s="5" t="s">
         <v>350</v>
@@ -4706,7 +4703,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="358" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A358" s="4">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B358" s="5" t="s">
         <v>351</v>
@@ -4714,7 +4711,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="359" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A359" s="4">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B359" s="5" t="s">
         <v>352</v>
@@ -4722,7 +4719,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="360" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A360" s="4">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B360" s="5" t="s">
         <v>353</v>
@@ -4730,7 +4727,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="361" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A361" s="4">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B361" s="5" t="s">
         <v>354</v>
@@ -4738,7 +4735,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="362" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A362" s="4">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B362" s="5" t="s">
         <v>355</v>
@@ -4746,7 +4743,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="363" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A363" s="4">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B363" s="5" t="s">
         <v>356</v>
@@ -4754,7 +4751,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="364" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A364" s="4">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B364" s="5" t="s">
         <v>357</v>
@@ -4762,7 +4759,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="365" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A365" s="4">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B365" s="5" t="s">
         <v>358</v>
@@ -4770,7 +4767,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="366" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A366" s="4">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B366" s="5" t="s">
         <v>359</v>
@@ -4778,7 +4775,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="367" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A367" s="4">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B367" s="5" t="s">
         <v>360</v>
@@ -4786,7 +4783,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="368" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A368" s="4">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B368" s="5" t="s">
         <v>361</v>
@@ -4794,7 +4791,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="369" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A369" s="4">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B369" s="5" t="s">
         <v>362</v>
@@ -4802,7 +4799,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="370" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A370" s="4">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B370" s="5" t="s">
         <v>363</v>
@@ -4810,7 +4807,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="371" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A371" s="4">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B371" s="5" t="s">
         <v>364</v>
@@ -4818,7 +4815,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="372" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A372" s="4">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B372" s="5" t="s">
         <v>365</v>
@@ -4826,7 +4823,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="373" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A373" s="4">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B373" s="5" t="s">
         <v>366</v>
@@ -4834,7 +4831,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="374" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A374" s="4">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B374" s="5" t="s">
         <v>367</v>
@@ -4842,7 +4839,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="375" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A375" s="4">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B375" s="5" t="s">
         <v>368</v>
@@ -4850,7 +4847,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="376" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A376" s="4">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B376" s="5" t="s">
         <v>369</v>
@@ -4858,7 +4855,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="377" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A377" s="4">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B377" s="5" t="s">
         <v>370</v>
@@ -4866,7 +4863,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="378" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A378" s="4">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B378" s="5" t="s">
         <v>371</v>
@@ -4874,7 +4871,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="379" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A379" s="4">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B379" s="5" t="s">
         <v>372</v>
@@ -4882,7 +4879,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="380" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A380" s="4">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B380" s="5" t="s">
         <v>373</v>
@@ -4890,15 +4887,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="381" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A381" s="4">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B381" s="5" t="s">
-        <v>374</v>
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="382" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A382" s="4">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B382" s="5" t="s">
         <v>2</v>
@@ -4906,15 +4903,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="383" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A383" s="4">
-        <v>459</v>
+        <v>491</v>
       </c>
       <c r="B383" s="5" t="s">
-        <v>2</v>
+        <v>374</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="384" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A384" s="4">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B384" s="5" t="s">
         <v>375</v>
@@ -4922,7 +4919,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="385" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A385" s="4">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B385" s="5" t="s">
         <v>376</v>
@@ -4930,7 +4927,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="386" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A386" s="4">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B386" s="5" t="s">
         <v>377</v>
@@ -4938,7 +4935,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="387" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A387" s="4">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B387" s="5" t="s">
         <v>378</v>
@@ -4946,7 +4943,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="388" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A388" s="4">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B388" s="5" t="s">
         <v>379</v>
@@ -4954,7 +4951,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="389" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A389" s="4">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B389" s="5" t="s">
         <v>380</v>
@@ -4962,7 +4959,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="390" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A390" s="4">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B390" s="5" t="s">
         <v>381</v>
@@ -4970,7 +4967,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="391" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A391" s="4">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B391" s="5" t="s">
         <v>382</v>
@@ -4978,7 +4975,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="392" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A392" s="4">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B392" s="5" t="s">
         <v>383</v>
@@ -4986,7 +4983,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="393" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A393" s="4">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B393" s="5" t="s">
         <v>384</v>
@@ -4994,7 +4991,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="394" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A394" s="4">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B394" s="5" t="s">
         <v>385</v>
@@ -5002,7 +4999,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="395" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A395" s="4">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B395" s="5" t="s">
         <v>386</v>
@@ -5010,7 +5007,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="396" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A396" s="4">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B396" s="5" t="s">
         <v>387</v>
@@ -5018,7 +5015,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="397" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A397" s="4">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B397" s="5" t="s">
         <v>388</v>
@@ -5026,7 +5023,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="398" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A398" s="4">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B398" s="5" t="s">
         <v>389</v>
@@ -5034,7 +5031,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="399" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A399" s="4">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B399" s="5" t="s">
         <v>390</v>
@@ -5042,7 +5039,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="400" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A400" s="4">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B400" s="5" t="s">
         <v>391</v>
@@ -5050,7 +5047,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="401" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A401" s="4">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B401" s="5" t="s">
         <v>392</v>
@@ -5058,7 +5055,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="402" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A402" s="4">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B402" s="5" t="s">
         <v>393</v>
@@ -5066,7 +5063,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="403" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A403" s="4">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B403" s="5" t="s">
         <v>394</v>
@@ -5074,7 +5071,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="404" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A404" s="4">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B404" s="5" t="s">
         <v>395</v>
@@ -5082,7 +5079,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="405" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A405" s="4">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B405" s="5" t="s">
         <v>396</v>
@@ -5090,7 +5087,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="406" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A406" s="4">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B406" s="5" t="s">
         <v>397</v>
@@ -5098,7 +5095,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="407" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A407" s="4">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B407" s="5" t="s">
         <v>398</v>
@@ -5106,7 +5103,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="408" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A408" s="4">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B408" s="5" t="s">
         <v>399</v>
@@ -5114,7 +5111,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="409" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A409" s="4">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B409" s="5" t="s">
         <v>400</v>
@@ -5122,7 +5119,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="410" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A410" s="4">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B410" s="5" t="s">
         <v>401</v>
@@ -5130,7 +5127,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="411" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A411" s="4">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B411" s="5" t="s">
         <v>402</v>
@@ -5138,7 +5135,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="412" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A412" s="4">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B412" s="5" t="s">
         <v>403</v>
@@ -5146,7 +5143,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="413" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A413" s="4">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B413" s="5" t="s">
         <v>404</v>
@@ -5154,7 +5151,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="414" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A414" s="4">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B414" s="5" t="s">
         <v>405</v>
@@ -5162,7 +5159,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="415" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A415" s="4">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B415" s="5" t="s">
         <v>406</v>
@@ -5170,7 +5167,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="416" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A416" s="4">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B416" s="5" t="s">
         <v>407</v>
@@ -5178,7 +5175,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="417" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A417" s="4">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B417" s="5" t="s">
         <v>408</v>
@@ -5186,7 +5183,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="418" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A418" s="4">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B418" s="5" t="s">
         <v>409</v>
@@ -5194,7 +5191,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="419" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A419" s="4">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B419" s="5" t="s">
         <v>410</v>
@@ -5202,7 +5199,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="420" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A420" s="4">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B420" s="5" t="s">
         <v>411</v>
@@ -5210,7 +5207,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="421" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A421" s="4">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B421" s="5" t="s">
         <v>412</v>
@@ -5218,7 +5215,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="422" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A422" s="4">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B422" s="5" t="s">
         <v>413</v>
@@ -5226,7 +5223,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="423" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A423" s="4">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B423" s="5" t="s">
         <v>414</v>
@@ -5234,7 +5231,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="424" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A424" s="4">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B424" s="5" t="s">
         <v>415</v>
@@ -5242,7 +5239,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="425" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A425" s="4">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B425" s="5" t="s">
         <v>416</v>
@@ -5250,7 +5247,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="426" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A426" s="4">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B426" s="5" t="s">
         <v>417</v>
@@ -5258,7 +5255,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="427" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A427" s="4">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B427" s="5" t="s">
         <v>418</v>
@@ -5266,7 +5263,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="428" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A428" s="4">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B428" s="5" t="s">
         <v>419</v>
@@ -5274,7 +5271,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="429" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A429" s="4">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B429" s="5" t="s">
         <v>420</v>
@@ -5282,7 +5279,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="430" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A430" s="4">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B430" s="5" t="s">
         <v>421</v>
@@ -5290,7 +5287,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="431" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A431" s="4">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B431" s="5" t="s">
         <v>422</v>
@@ -5298,7 +5295,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="432" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A432" s="4">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B432" s="5" t="s">
         <v>423</v>
@@ -5306,7 +5303,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="433" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A433" s="4">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B433" s="5" t="s">
         <v>424</v>
@@ -5314,7 +5311,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="434" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A434" s="4">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B434" s="5" t="s">
         <v>425</v>
@@ -5322,7 +5319,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="435" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A435" s="4">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B435" s="5" t="s">
         <v>426</v>
@@ -5330,7 +5327,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="436" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A436" s="4">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B436" s="5" t="s">
         <v>427</v>
@@ -5338,7 +5335,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="437" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A437" s="4">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B437" s="5" t="s">
         <v>428</v>
@@ -5346,7 +5343,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="438" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A438" s="4">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B438" s="5" t="s">
         <v>429</v>
@@ -5354,7 +5351,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="439" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A439" s="4">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B439" s="5" t="s">
         <v>430</v>
@@ -5362,7 +5359,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="440" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A440" s="4">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B440" s="5" t="s">
         <v>431</v>
@@ -5370,7 +5367,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="441" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A441" s="4">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="B441" s="5" t="s">
         <v>432</v>
@@ -5378,7 +5375,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="442" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A442" s="4">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B442" s="5" t="s">
         <v>433</v>
@@ -5386,7 +5383,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="443" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A443" s="4">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B443" s="5" t="s">
         <v>434</v>
@@ -5394,7 +5391,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="444" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A444" s="4">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B444" s="5" t="s">
         <v>435</v>
@@ -5402,15 +5399,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="445" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A445" s="4">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B445" s="5" t="s">
-        <v>436</v>
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="446" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A446" s="4">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B446" s="5" t="s">
         <v>2</v>
@@ -5418,31 +5415,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="447" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A447" s="4">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B447" s="5" t="s">
-        <v>2</v>
+        <v>436</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="448" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A448" s="4">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B448" s="5" t="s">
-        <v>437</v>
+        <v>172</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="449" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A449" s="4">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B449" s="5" t="s">
-        <v>173</v>
+        <v>437</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="450" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A450" s="4">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B450" s="5" t="s">
         <v>438</v>
@@ -5450,7 +5447,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="451" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A451" s="4">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B451" s="5" t="s">
         <v>439</v>
@@ -5458,7 +5455,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="452" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A452" s="4">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B452" s="5" t="s">
         <v>440</v>
@@ -5466,39 +5463,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="453" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A453" s="4">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="B453" s="5" t="s">
-        <v>441</v>
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="454" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A454" s="4">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="B454" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="455" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A455" s="4">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="B455" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="456" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A456" s="4">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B456" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="457" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A457" s="4">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B457" s="5" t="s">
         <v>5</v>
@@ -5506,15 +5503,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="458" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A458" s="4">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B458" s="5" t="s">
-        <v>5</v>
+        <v>441</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="459" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A459" s="4">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B459" s="5" t="s">
         <v>442</v>
@@ -5522,7 +5519,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="460" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A460" s="4">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="B460" s="5" t="s">
         <v>443</v>
@@ -5530,7 +5527,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="461" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A461" s="4">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B461" s="5" t="s">
         <v>444</v>
@@ -5538,7 +5535,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="462" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A462" s="4">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="B462" s="5" t="s">
         <v>445</v>
@@ -5546,7 +5543,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="463" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A463" s="4">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B463" s="5" t="s">
         <v>446</v>
@@ -5554,7 +5551,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="464" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A464" s="4">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B464" s="5" t="s">
         <v>447</v>
@@ -5562,7 +5559,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="465" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A465" s="4">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="B465" s="5" t="s">
         <v>448</v>
@@ -5570,23 +5567,23 @@
     </row>
     <row x14ac:dyDescent="0.25" r="466" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A466" s="4">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="467" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A467" s="4">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="468" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A468" s="4">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B468" s="5" t="s">
         <v>438</v>
@@ -5594,7 +5591,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="469" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A469" s="4">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B469" s="5" t="s">
         <v>439</v>
@@ -5602,63 +5599,63 @@
     </row>
     <row x14ac:dyDescent="0.25" r="470" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A470" s="4">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="471" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A471" s="4">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="472" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A472" s="4">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="473" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A473" s="4">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="474" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A474" s="4">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="475" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A475" s="4">
-        <v>620</v>
+        <v>584</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>437</v>
+        <v>451</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="476" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A476" s="4">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="B476" s="5" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="477" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A477" s="4">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="B477" s="5" t="s">
         <v>450</v>
@@ -5666,15 +5663,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="478" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A478" s="4">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="479" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A479" s="4">
-        <v>597</v>
+        <v>607</v>
       </c>
       <c r="B479" s="5" t="s">
         <v>453</v>
@@ -5682,7 +5679,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="480" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A480" s="4">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="B480" s="5" t="s">
         <v>454</v>
@@ -5690,7 +5687,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="481" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A481" s="4">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B481" s="5" t="s">
         <v>455</v>
@@ -5698,23 +5695,23 @@
     </row>
     <row x14ac:dyDescent="0.25" r="482" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A482" s="4">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="483" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A483" s="4">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B483" s="5" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="484" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A484" s="4">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="B484" s="5" t="s">
         <v>457</v>
@@ -5722,7 +5719,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="485" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A485" s="4">
-        <v>618</v>
+        <v>625</v>
       </c>
       <c r="B485" s="5" t="s">
         <v>458</v>
@@ -5730,39 +5727,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="486" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A486" s="4">
-        <v>625</v>
+        <v>585</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="487" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A487" s="4">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="488" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A488" s="4">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="489" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A489" s="4">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="490" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A490" s="4">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="B490" s="5" t="s">
         <v>456</v>
@@ -5770,87 +5767,87 @@
     </row>
     <row x14ac:dyDescent="0.25" r="491" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A491" s="4">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="492" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A492" s="4">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="493" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A493" s="4">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="494" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A494" s="4">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>437</v>
+        <v>172</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="495" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A495" s="4">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>173</v>
+        <v>444</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="496" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A496" s="4">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="497" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A497" s="4">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B497" s="5" t="s">
-        <v>447</v>
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="498" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A498" s="4">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>2</v>
+        <v>439</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="499" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A499" s="4">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>440</v>
+        <v>172</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="500" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A500" s="4">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>173</v>
+        <v>458</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="501" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A501" s="4">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B501" s="5" t="s">
         <v>459</v>
@@ -5858,19 +5855,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="502" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A502" s="4">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B502" s="5" t="s">
         <v>460</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="503" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A503" s="4">
-        <v>626</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>461</v>
-      </c>
+      <c r="A503" s="6"/>
+      <c r="B503" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="504" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A504" s="6"/>
@@ -7851,10 +7844,6 @@
     <row x14ac:dyDescent="0.25" r="998" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A998" s="6"/>
       <c r="B998" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="999" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A999" s="6"/>
-      <c r="B999" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>